<commit_message>
Add new file to directory
</commit_message>
<xml_diff>
--- a/ExcelCo/basics/03_edit_mode.xlsx
+++ b/ExcelCo/basics/03_edit_mode.xlsx
@@ -48,9 +48,6 @@
     <t>Sacramento</t>
   </si>
   <si>
-    <t>2. Then using F2 / CTRL+U, toggle to formula mode and navigate to the cell with the corresponding state capital</t>
-  </si>
-  <si>
     <t>1. In each of the grey boxes below, enter the cell (using Lesson 1's learnings) and delete all of the text after the "&amp;" sign</t>
   </si>
   <si>
@@ -100,6 +97,9 @@
   </si>
   <si>
     <t>He took the [time of day] [mode of transport]</t>
+  </si>
+  <si>
+    <t>2. Then using F2 / CTRL+U, toggle to formula mode and navigate to the cell with the corresponding state capital (they're not in order)</t>
   </si>
 </sst>
 </file>
@@ -990,7 +990,7 @@
   <dimension ref="B1:N21"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1181,7 +1181,7 @@
     <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D12" s="11"/>
       <c r="E12" s="7"/>
@@ -1196,7 +1196,7 @@
     <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="20" t="s">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
@@ -1464,14 +1464,14 @@
   <sheetData>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="37" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C3" s="37"/>
       <c r="D3" s="35"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" s="29"/>
       <c r="D4" s="36"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="29"/>
       <c r="D5" s="36"/>
@@ -1493,7 +1493,7 @@
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C6" s="29"/>
       <c r="D6" s="36"/>
@@ -1504,7 +1504,7 @@
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="21" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C7" s="29"/>
       <c r="D7" s="36"/>
@@ -1515,7 +1515,7 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="29"/>
       <c r="D8" s="36"/>
@@ -1526,7 +1526,7 @@
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C9" s="29"/>
       <c r="D9" s="36"/>
@@ -1537,21 +1537,21 @@
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="37" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C11" s="37"/>
       <c r="D11" s="35"/>
     </row>
     <row r="13" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B13" s="37" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C13" s="37"/>
       <c r="D13" s="35"/>
     </row>
     <row r="14" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B14" s="33" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="34"/>
       <c r="D14" s="36"/>
@@ -1567,7 +1567,7 @@
     </row>
     <row r="15" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B15" s="33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C15" s="34"/>
       <c r="D15" s="36"/>
@@ -1583,7 +1583,7 @@
     </row>
     <row r="16" spans="2:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B16" s="33" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C16" s="34"/>
       <c r="D16" s="36"/>
@@ -1603,18 +1603,18 @@
     </row>
     <row r="17" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B17" s="33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17" s="34"/>
       <c r="D17" s="36"/>
       <c r="G17" s="31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H17" s="31"/>
     </row>
     <row r="18" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B18" s="33" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="34"/>
       <c r="D18" s="36"/>
@@ -1630,7 +1630,7 @@
     </row>
     <row r="19" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B19" s="33" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="34"/>
       <c r="D19" s="36"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="20" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B20" s="33" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C20" s="34"/>
       <c r="D20" s="36"/>
@@ -1666,12 +1666,12 @@
     </row>
     <row r="21" spans="2:14" hidden="1" outlineLevel="1" x14ac:dyDescent="0.2">
       <c r="B21" s="33" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C21" s="34"/>
       <c r="D21" s="36"/>
       <c r="G21" s="31" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H21" s="31"/>
     </row>

</xml_diff>